<commit_message>
Members Area, my feedback E2E Completed
</commit_message>
<xml_diff>
--- a/Data Files/Members_Data.xlsx
+++ b/Data Files/Members_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49D61D6-EE08-43CF-B940-1DD83B20E253}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C38104-D1BC-419B-93D5-58B9C251391C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20580" yWindow="-60" windowWidth="20640" windowHeight="13200" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView xWindow="2205" yWindow="2505" windowWidth="31095" windowHeight="11385" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,19 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>tradeLocationVerification</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>X_COORD</t>
-  </si>
-  <si>
-    <t>Y_COORD</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -79,13 +67,61 @@
   </si>
   <si>
     <t>Trouble logging in?</t>
+  </si>
+  <si>
+    <t>customer_Town</t>
+  </si>
+  <si>
+    <t>Chichester</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>returned_Search_Head</t>
+  </si>
+  <si>
+    <t>returned_Search_Comment</t>
+  </si>
+  <si>
+    <t>loft extension</t>
+  </si>
+  <si>
+    <t>I would recommend this company and</t>
+  </si>
+  <si>
+    <t>customer_Surname</t>
+  </si>
+  <si>
+    <t>returned_Work_Done_Date</t>
+  </si>
+  <si>
+    <t>Work done: Oct 2018</t>
+  </si>
+  <si>
+    <t>returned_Feedback_Status</t>
+  </si>
+  <si>
+    <t>Feedback Published</t>
+  </si>
+  <si>
+    <t>customer_Email</t>
+  </si>
+  <si>
+    <t>Customer_Phone</t>
+  </si>
+  <si>
+    <t>feedback@panic.com</t>
+  </si>
+  <si>
+    <t>07788123456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +134,26 @@
       <color rgb="FF212529"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,10 +173,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -129,8 +186,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,13 +505,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56B88-33E9-468B-853E-05EE5D8A6600}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD10"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
@@ -457,68 +519,111 @@
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="47.140625" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="31.28515625" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{BE961D19-B2B0-4D95-9534-58692B5B8E6F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on Members->My Profile Functionality
</commit_message>
<xml_diff>
--- a/Data Files/Members_Data.xlsx
+++ b/Data Files/Members_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C38104-D1BC-419B-93D5-58B9C251391C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921C63F6-CBA3-4E80-82BA-1E22A6A87741}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2505" windowWidth="31095" windowHeight="11385" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Username</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>07788123456</t>
+  </si>
+  <si>
+    <t>MEMBER_ID</t>
   </si>
 </sst>
 </file>
@@ -505,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56B88-33E9-468B-853E-05EE5D8A6600}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,7 +534,7 @@
     <col min="16" max="16" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,8 +577,11 @@
       <c r="N1" t="s">
         <v>22</v>
       </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="17.25">
+    <row r="2" spans="1:15" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -617,6 +623,9 @@
       </c>
       <c r="N2" t="s">
         <v>23</v>
+      </c>
+      <c r="O2" s="2">
+        <v>218630</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Console based test execution updates
</commit_message>
<xml_diff>
--- a/Data Files/Members_Data.xlsx
+++ b/Data Files/Members_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921C63F6-CBA3-4E80-82BA-1E22A6A87741}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF3480-1FE3-4F0A-B503-FED0E83316A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
@@ -124,7 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,15 +510,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56B88-33E9-468B-853E-05EE5D8A6600}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
@@ -534,7 +534,7 @@
     <col min="16" max="16" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17.25">
+    <row r="2" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Adding test coverage - Web Office->Settings->Members Area - 11 Tests - 10% Complete
Also, Members Area My_Profile and My Feedback, Dev changes factored into
failing tests
</commit_message>
<xml_diff>
--- a/Data Files/Members_Data.xlsx
+++ b/Data Files/Members_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\git\src\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF3480-1FE3-4F0A-B503-FED0E83316A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E43043-0F34-485D-97FA-E24CDD310031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,30 +75,18 @@
     <t>Chichester</t>
   </si>
   <si>
-    <t>Feedback</t>
-  </si>
-  <si>
     <t>returned_Search_Head</t>
   </si>
   <si>
     <t>returned_Search_Comment</t>
   </si>
   <si>
-    <t>loft extension</t>
-  </si>
-  <si>
-    <t>I would recommend this company and</t>
-  </si>
-  <si>
     <t>customer_Surname</t>
   </si>
   <si>
     <t>returned_Work_Done_Date</t>
   </si>
   <si>
-    <t>Work done: Oct 2018</t>
-  </si>
-  <si>
     <t>returned_Feedback_Status</t>
   </si>
   <si>
@@ -118,6 +106,18 @@
   </si>
   <si>
     <t>MEMBER_ID</t>
+  </si>
+  <si>
+    <t>Work done</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Testing references</t>
+  </si>
+  <si>
+    <t>Aware of feedback</t>
   </si>
 </sst>
 </file>
@@ -139,12 +139,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF212529"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
@@ -157,6 +151,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,7 +178,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -189,10 +189,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -510,31 +510,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56B88-33E9-468B-853E-05EE5D8A6600}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.265625" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" customWidth="1"/>
+    <col min="3" max="3" width="57.73046875" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" customWidth="1"/>
+    <col min="5" max="5" width="20.59765625" customWidth="1"/>
+    <col min="6" max="6" width="21.1328125" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.73046875" customWidth="1"/>
+    <col min="10" max="10" width="17.86328125" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" customWidth="1"/>
-    <col min="14" max="14" width="31.28515625" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="28.3984375" customWidth="1"/>
+    <col min="13" max="13" width="24.3984375" customWidth="1"/>
+    <col min="14" max="14" width="31.265625" customWidth="1"/>
+    <col min="15" max="15" width="23.73046875" customWidth="1"/>
+    <col min="16" max="16" width="21.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,34 +554,34 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
       </c>
       <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.7">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -601,28 +601,28 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>21</v>
+      <c r="L2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O2" s="2">
         <v>218630</v>

</xml_diff>